<commit_message>
Creación de funciones PWM Y MAP
Se utilizaron la función de MAP Para poder hacer una equivalencia de un valor de 0 a 1023 de resolución del ADC a una resolución de 8 bits
</commit_message>
<xml_diff>
--- a/PinoutLab6.xlsx
+++ b/PinoutLab6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\LABS\LAB5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4896F2F-0FE9-405D-8AFB-0132BF2EE819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74430CB3-D97F-4305-9C4F-6FF3D74AC9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Entradas</t>
   </si>
@@ -163,6 +163,30 @@
   </si>
   <si>
     <t>GPIO12</t>
+  </si>
+  <si>
+    <t>LED ROJA</t>
+  </si>
+  <si>
+    <t>LED VERDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED AMARILLA </t>
+  </si>
+  <si>
+    <t>GPIO4</t>
+  </si>
+  <si>
+    <t>GPIO2</t>
+  </si>
+  <si>
+    <t>GPIO15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED VERDE </t>
+  </si>
+  <si>
+    <t>LED AMARILLA</t>
   </si>
 </sst>
 </file>
@@ -194,7 +218,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +255,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -244,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -269,6 +299,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,7 +822,7 @@
   <dimension ref="A3:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J13" sqref="J13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,7 +1021,9 @@
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
@@ -1009,6 +1042,9 @@
       <c r="I14" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="J14" s="14" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
@@ -1026,6 +1062,9 @@
       <c r="I15" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="J15" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
@@ -1046,8 +1085,12 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1059,8 +1102,12 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1068,8 +1115,12 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>

</xml_diff>

<commit_message>
arreglo de variable contador
</commit_message>
<xml_diff>
--- a/PinoutLab6.xlsx
+++ b/PinoutLab6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\SEMESTRE DE LA U\6TO SEMESTRE\DIGITAL 2\LABS\LAB5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74430CB3-D97F-4305-9C4F-6FF3D74AC9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D296AB-85C1-4230-8E1C-1EF27978480A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33FA0D3F-264E-4F2D-8D17-345DFAF046CD}"/>
   </bookViews>
@@ -296,10 +296,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,7 +822,7 @@
   <dimension ref="A3:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:J15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,10 +843,10 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -933,15 +933,12 @@
       <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
@@ -956,9 +953,6 @@
       <c r="I10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1021,7 +1015,7 @@
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1033,7 +1027,9 @@
       <c r="C14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1042,7 +1038,7 @@
       <c r="I14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1053,7 +1049,9 @@
       <c r="C15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1062,7 +1060,7 @@
       <c r="I15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="13" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1085,10 +1083,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -1102,10 +1100,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="3"/>
@@ -1115,10 +1113,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F19" s="3"/>

</xml_diff>